<commit_message>
Update data files - Bot run at 2026-02-12 08:55:12 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -1161,9 +1161,13 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>1</v>
-      </c>
-      <c r="E14" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2026-02-12T08:55:06.170253+00:00</t>
+        </is>
+      </c>
       <c r="F14" t="inlineStr">
         <is>
           <t>['08:24-09:26']</t>
@@ -1173,7 +1177,7 @@
         <v>0</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
@@ -1188,7 +1192,7 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[21, 24, 17]</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-13 06:05:51 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -953,9 +953,13 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2026-02-13T06:05:46.135770+00:00</t>
+        </is>
+      </c>
       <c r="F10" t="inlineStr">
         <is>
           <t>['05:36-06:38']</t>
@@ -965,7 +969,7 @@
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I10" t="n">
         <v>0</v>
@@ -980,7 +984,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[31, 15, 39, 5]</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-13 07:33:00 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -1556,7 +1556,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>2026-02-13T07:27:50.964363+00:00</t>
+          <t>2026-02-13T07:32:55.202461+00:00</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1568,7 +1568,7 @@
         <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I21" t="n">
         <v>2</v>
@@ -1583,7 +1583,7 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>[19, 32]</t>
+          <t>[19, 32, 25, 15]</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-13 13:11:25 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -1943,11 +1943,11 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>2026-02-12T18:31:27.453512+00:00</t>
+          <t>2026-02-13T13:11:20.494625+00:00</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -1959,7 +1959,7 @@
         <v>0</v>
       </c>
       <c r="H28" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I28" t="n">
         <v>0</v>
@@ -1974,7 +1974,7 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>[19733, 19735, 19728]</t>
+          <t>[19733, 19735, 19728, 24545, 24552]</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-13 23:49:34 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -422,67 +434,67 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>username</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>group_name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>join_date</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>current_phase</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>last_action_date</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>time_ranges</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>link_enabled</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>reactions_count</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>replies_count</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>posts_count</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>status</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>reacted_message_ids</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>replied_message_ids</t>
         </is>
@@ -723,7 +735,11 @@
       <c r="D6" t="n">
         <v>1</v>
       </c>
-      <c r="E6" t="inlineStr"/>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2026-02-13T23:49:27.876231+00:00</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
           <t>['23:20-24:00']</t>
@@ -733,7 +749,7 @@
         <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -748,7 +764,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[138845, 138840, 138838]</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-14 07:23:07 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -1216,7 +1216,11 @@
       <c r="D15" t="n">
         <v>1</v>
       </c>
-      <c r="E15" t="inlineStr"/>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2026-02-14T07:23:03.045004+00:00</t>
+        </is>
+      </c>
       <c r="F15" t="inlineStr">
         <is>
           <t>['07:20-08:00']</t>
@@ -1226,7 +1230,7 @@
         <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
@@ -1241,7 +1245,7 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[140]</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-14 09:51:52 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -1379,7 +1379,11 @@
       <c r="D18" t="n">
         <v>1</v>
       </c>
-      <c r="E18" t="inlineStr"/>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2026-02-14T09:51:46.517739+00:00</t>
+        </is>
+      </c>
       <c r="F18" t="inlineStr">
         <is>
           <t>['09:20-10:00']</t>
@@ -1389,7 +1393,7 @@
         <v>0</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I18" t="n">
         <v>0</v>
@@ -1404,7 +1408,7 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[14787, 14732]</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-14 10:57:34 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -845,7 +845,11 @@
       <c r="D8" t="n">
         <v>1</v>
       </c>
-      <c r="E8" t="inlineStr"/>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2026-02-14T10:57:30.037964+00:00</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>['10:50-11:40']</t>
@@ -855,7 +859,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
@@ -870,7 +874,7 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[67725, 67732]</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-14 13:56:34 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -1008,7 +1008,11 @@
       <c r="D11" t="n">
         <v>1</v>
       </c>
-      <c r="E11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2026-02-14T13:56:29.483534+00:00</t>
+        </is>
+      </c>
       <c r="F11" t="inlineStr">
         <is>
           <t>['13:20-14:10']</t>
@@ -1018,7 +1022,7 @@
         <v>0</v>
       </c>
       <c r="H11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
@@ -1033,7 +1037,7 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[68028, 68030]</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">

</xml_diff>

<commit_message>
Update data files - Bot run at 2026-02-14 17:53:42 UTC
</commit_message>
<xml_diff>
--- a/group_promotion_service/data/groups_progress.xlsx
+++ b/group_promotion_service/data/groups_progress.xlsx
@@ -521,7 +521,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2026-02-14T17:00:59.092207+00:00</t>
+          <t>2026-02-14T17:53:38.523130+00:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -533,7 +533,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I2" t="n">
         <v>0</v>
@@ -548,7 +548,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[272297, 272284]</t>
+          <t>[272297, 272284, 272295, 272300, 272286]</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">

</xml_diff>